<commit_message>
All updates before first test
</commit_message>
<xml_diff>
--- a/Catheter properties.xlsx
+++ b/Catheter properties.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Catheter code</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Heat Time</t>
-  </si>
-  <si>
-    <t>Xi (distance between pin wall to catheter wall)</t>
   </si>
   <si>
     <t>Yi (Dist end of grippers to bending pin)</t>
@@ -595,26 +592,26 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -640,14 +637,11 @@
       <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -655,7 +649,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="8">
         <v>4.25</v>
@@ -667,22 +661,23 @@
         <v>1.98</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" s="10"/>
       <c r="I2" s="11">
         <v>0.5</v>
       </c>
-      <c r="J2" s="10"/>
+      <c r="J2" s="10">
+        <v>0.5</v>
+      </c>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="14">
         <v>42</v>
@@ -694,23 +689,26 @@
         <v>1.17</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
+      <c r="I3" s="16">
+        <v>2</v>
+      </c>
+      <c r="J3" s="10">
+        <v>0.5</v>
+      </c>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="14">
-        <v>711.2</v>
+        <v>100</v>
       </c>
       <c r="E4" s="14">
         <v>1.67</v>
@@ -719,50 +717,75 @@
         <v>1.17</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
+      <c r="I4" s="16">
+        <v>2</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.5</v>
+      </c>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="D5" s="16">
+        <v>50</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1.67</v>
+      </c>
+      <c r="F5" s="16">
+        <v>1.17</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
+      <c r="I5" s="16">
+        <v>4</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.5</v>
+      </c>
       <c r="K5" s="16"/>
       <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="D6" s="18">
+        <v>50</v>
+      </c>
+      <c r="E6" s="18">
+        <v>1.33</v>
+      </c>
+      <c r="F6" s="18">
+        <v>1.17</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+      <c r="I6" s="18">
+        <v>4</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.5</v>
+      </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -770,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="8">
         <v>4.25</v>
@@ -782,7 +805,7 @@
         <v>1.98</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="11">
@@ -791,13 +814,12 @@
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="14">
         <v>42</v>
@@ -809,20 +831,19 @@
         <v>1.17</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" s="16"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="14">
         <v>711.2</v>
@@ -834,33 +855,43 @@
         <v>1.17</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="16">
+        <v>50</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1.67</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1.17</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16">
+        <v>4</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -868,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="8">
         <v>4.25</v>
@@ -880,7 +911,7 @@
         <v>1.98</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="11">
@@ -889,13 +920,12 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" s="14">
         <v>42</v>
@@ -907,20 +937,19 @@
         <v>1.17</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
       <c r="C13" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="21">
         <v>711.2</v>
@@ -932,16 +961,15 @@
         <v>1.17</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>4</v>
       </c>
@@ -949,7 +977,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" s="8">
         <v>4.25</v>
@@ -961,7 +989,7 @@
         <v>1.98</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="11">
@@ -970,13 +998,12 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="14">
         <v>42</v>
@@ -988,16 +1015,15 @@
         <v>1.17</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="23">
         <v>5</v>
       </c>
@@ -1005,7 +1031,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D16" s="26">
         <v>4.25</v>
@@ -1017,7 +1043,7 @@
         <v>1.98</v>
       </c>
       <c r="G16" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="29">
@@ -1026,13 +1052,12 @@
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
       <c r="C17" s="31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" s="32">
         <v>42</v>
@@ -1044,20 +1069,19 @@
         <v>1.17</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="34"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="35"/>
       <c r="C18" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" s="37">
         <v>711.2</v>
@@ -1069,14 +1093,13 @@
         <v>1.17</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
       <c r="J18" s="39"/>
       <c r="K18" s="39"/>
       <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
main.py updated to latest
</commit_message>
<xml_diff>
--- a/Catheter properties.xlsx
+++ b/Catheter properties.xlsx
@@ -112,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -209,11 +209,155 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF303336"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF303336"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF303336"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF303336"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF303336"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF303336"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF303336"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF303336"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF303336"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -251,12 +395,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -288,6 +426,19 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +743,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -641,7 +792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -673,7 +824,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13" t="s">
@@ -695,13 +846,13 @@
       <c r="I3" s="16">
         <v>2</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="16">
         <v>0.5</v>
       </c>
       <c r="K3" s="16"/>
       <c r="L3" s="16"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="13"/>
       <c r="C4" s="13" t="s">
@@ -723,13 +874,13 @@
       <c r="I4" s="16">
         <v>2</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="16">
         <v>0.5</v>
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
@@ -751,7 +902,7 @@
       <c r="I5" s="16">
         <v>4</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="16">
         <v>0.5</v>
       </c>
       <c r="K5" s="16"/>
@@ -779,13 +930,13 @@
       <c r="I6" s="18">
         <v>4</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="16">
         <v>0.5</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -817,7 +968,7 @@
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="13" t="s">
@@ -839,13 +990,13 @@
       <c r="I8" s="16">
         <v>2</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="16">
         <v>0.5</v>
       </c>
       <c r="K8" s="16"/>
       <c r="L8" s="16"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="13" t="s">
@@ -867,7 +1018,7 @@
       <c r="I9" s="16">
         <v>2</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="16">
         <v>0.5</v>
       </c>
       <c r="K9" s="16"/>
@@ -879,29 +1030,29 @@
       <c r="C10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="16">
+      <c r="D10" s="39">
         <v>50</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="39">
         <v>1.67</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="39">
         <v>1.17</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16">
+      <c r="H10" s="39"/>
+      <c r="I10" s="39">
         <v>4</v>
       </c>
-      <c r="J10" s="10">
+      <c r="J10" s="16">
         <v>0.5</v>
       </c>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -911,20 +1062,20 @@
       <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="8">
-        <v>4.25</v>
-      </c>
-      <c r="E11" s="8">
+      <c r="D11" s="46">
+        <v>300</v>
+      </c>
+      <c r="E11" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="F11" s="43">
         <v>1.2</v>
       </c>
-      <c r="F11" s="9">
-        <v>1.98</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11">
+      <c r="H11" s="43"/>
+      <c r="I11" s="38">
         <v>0.5</v>
       </c>
       <c r="J11" s="10">
@@ -933,29 +1084,29 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="14">
-        <v>42</v>
-      </c>
-      <c r="E12" s="14">
-        <v>1.67</v>
-      </c>
-      <c r="F12" s="15">
+      <c r="D12" s="47">
+        <v>800</v>
+      </c>
+      <c r="E12" s="41">
+        <v>1.6</v>
+      </c>
+      <c r="F12" s="44">
         <v>1.17</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16">
-        <v>2</v>
-      </c>
-      <c r="J12" s="10">
+      <c r="H12" s="44"/>
+      <c r="I12" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="16">
         <v>0.5</v>
       </c>
       <c r="K12" s="16"/>
@@ -967,29 +1118,29 @@
       <c r="C13" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="48">
         <v>711.2</v>
       </c>
-      <c r="E13" s="21">
-        <v>1.67</v>
-      </c>
-      <c r="F13" s="22">
+      <c r="E13" s="42">
+        <v>1.6</v>
+      </c>
+      <c r="F13" s="45">
         <v>1.17</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18">
-        <v>2</v>
-      </c>
-      <c r="J13" s="10">
+      <c r="H13" s="45"/>
+      <c r="I13" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="J13" s="16">
         <v>0.5</v>
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>4</v>
       </c>
@@ -1043,99 +1194,126 @@
       <c r="I15" s="16">
         <v>4</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="16">
         <v>0.5</v>
       </c>
       <c r="K15" s="16"/>
       <c r="L15" s="16"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="21">
         <v>5</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <v>3</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="24">
         <v>4.25</v>
       </c>
-      <c r="E16" s="26">
+      <c r="E16" s="24">
         <v>1.2</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="25">
         <v>1.98</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="28"/>
-      <c r="I16" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="J16" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31" t="s">
+      <c r="H16" s="26"/>
+      <c r="I16" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J16" s="49">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="30">
         <v>42</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="30">
         <v>1.67</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="31">
         <v>1.17</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34">
+      <c r="H17" s="32"/>
+      <c r="I17" s="32">
         <v>4</v>
       </c>
-      <c r="J17" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
+      <c r="J17" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36" t="s">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="37">
+      <c r="D18" s="35">
         <v>711.2</v>
       </c>
-      <c r="E18" s="37">
+      <c r="E18" s="35">
         <v>1.67</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="36">
         <v>1.17</v>
       </c>
-      <c r="G18" s="36" t="s">
+      <c r="G18" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39">
+      <c r="H18" s="37"/>
+      <c r="I18" s="37">
         <v>4</v>
       </c>
-      <c r="J18" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
+      <c r="J18" s="50">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="38"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>